<commit_message>
updated design for the database
</commit_message>
<xml_diff>
--- a/assets/design/database.xlsx
+++ b/assets/design/database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -44,12 +44,6 @@
     <t>varchar(255) not null</t>
   </si>
   <si>
-    <t>date_time</t>
-  </si>
-  <si>
-    <t>timestamp not null</t>
-  </si>
-  <si>
     <t>human_impact</t>
   </si>
   <si>
@@ -165,13 +159,31 @@
   </si>
   <si>
     <t>EmbedOrganization</t>
+  </si>
+  <si>
+    <t>date not null</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Design Choice:</t>
+  </si>
+  <si>
+    <t>Links in text</t>
+  </si>
+  <si>
+    <t>Embeds in text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +193,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -270,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -279,6 +300,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,11 +581,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -575,19 +595,21 @@
     <col min="8" max="8" width="41.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="G1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="2"/>
+      <c r="G1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -600,14 +622,12 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -617,16 +637,16 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -639,10 +659,10 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="G4" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -653,388 +673,408 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
+      <c r="G5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>42</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>44</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="G8" s="3" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>45</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="G12" s="3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
+      <c r="G13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>46</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="6" t="s">
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="D19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="D26" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="D30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="B34" s="4"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4"/>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="D18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="D25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="4"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="4"/>
-      <c r="D29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>19</v>
+      <c r="B36" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated design for database citations
</commit_message>
<xml_diff>
--- a/assets/design/database.xlsx
+++ b/assets/design/database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="49">
   <si>
     <t>name</t>
   </si>
@@ -107,9 +107,6 @@
     <t>integer not null auto_increment primary key</t>
   </si>
   <si>
-    <t>citation</t>
-  </si>
-  <si>
     <t>CitationPerson</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
   </si>
   <si>
     <t>CitationOrganization</t>
-  </si>
-  <si>
-    <t>link</t>
   </si>
   <si>
     <t>linkID</t>
@@ -605,10 +599,10 @@
       </c>
       <c r="E1" s="2"/>
       <c r="G1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>48</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -625,7 +619,7 @@
         <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -637,7 +631,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>5</v>
@@ -659,10 +653,10 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="G4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -677,7 +671,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="G5" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>7</v>
@@ -685,10 +679,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
@@ -701,10 +695,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -713,7 +707,7 @@
         <v>17</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -727,10 +721,10 @@
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="G8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -741,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="3" t="s">
@@ -781,7 +775,7 @@
         <v>17</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -791,10 +785,10 @@
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="G12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -803,7 +797,7 @@
       </c>
       <c r="B13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="3" t="s">
@@ -843,7 +837,7 @@
         <v>17</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H15" s="4"/>
     </row>
@@ -855,10 +849,10 @@
         <v>5</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -869,10 +863,10 @@
         <v>5</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>19</v>
@@ -885,7 +879,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -909,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>5</v>
@@ -933,7 +927,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" s="4"/>
     </row>
@@ -945,7 +939,7 @@
         <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>25</v>
@@ -975,7 +969,7 @@
       </c>
       <c r="B26" s="2"/>
       <c r="D26" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="4"/>
     </row>
@@ -987,7 +981,7 @@
         <v>17</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>25</v>
@@ -1019,7 +1013,7 @@
       </c>
       <c r="B30" s="4"/>
       <c r="D30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E30" s="4"/>
     </row>
@@ -1031,7 +1025,7 @@
         <v>17</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
updated design of database, merged date and time for simpler sorting in future
</commit_message>
<xml_diff>
--- a/assets/design/database.xlsx
+++ b/assets/design/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>name</t>
   </si>
@@ -155,15 +155,6 @@
     <t>EmbedOrganization</t>
   </si>
   <si>
-    <t>date not null</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>Design Choice:</t>
   </si>
   <si>
@@ -171,6 +162,12 @@
   </si>
   <si>
     <t>Embeds in text</t>
+  </si>
+  <si>
+    <t>date_time</t>
+  </si>
+  <si>
+    <t>datetime not null</t>
   </si>
 </sst>
 </file>
@@ -575,9 +572,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -599,10 +598,10 @@
       </c>
       <c r="E1" s="2"/>
       <c r="G1" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -679,10 +678,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
@@ -695,10 +694,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
@@ -713,7 +712,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -729,7 +728,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -747,7 +746,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -762,12 +761,8 @@
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="D11" s="3" t="s">
         <v>18</v>
       </c>
@@ -780,7 +775,9 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
+      <c r="A12" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
@@ -792,10 +789,12 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="4"/>
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
@@ -809,10 +808,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>24</v>
@@ -825,7 +824,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>5</v>
@@ -843,7 +842,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>5</v>
@@ -856,17 +855,13 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
       <c r="D17" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>19</v>
@@ -876,7 +871,9 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
+      <c r="A18" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="B18" s="4"/>
       <c r="D18" s="1" t="s">
         <v>28</v>
@@ -884,10 +881,12 @@
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="4"/>
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="D19" s="3" t="s">
         <v>1</v>
       </c>
@@ -897,10 +896,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>0</v>
@@ -911,7 +910,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>5</v>
@@ -921,7 +920,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>5</v>
@@ -931,11 +930,11 @@
       </c>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -946,12 +945,6 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="D24" s="3" t="s">
         <v>12</v>
       </c>
@@ -959,15 +952,21 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D26" s="5" t="s">
         <v>30</v>
       </c>
@@ -975,7 +974,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>17</v>
@@ -988,12 +987,8 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="D28" s="3" t="s">
         <v>18</v>
       </c>
@@ -1002,16 +997,20 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
+      <c r="A29" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="B29" s="4"/>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="4"/>
+      <c r="A30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D30" s="5" t="s">
         <v>31</v>
       </c>
@@ -1019,7 +1018,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>17</v>
@@ -1032,12 +1031,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
       <c r="D32" s="6" t="s">
         <v>19</v>
       </c>
@@ -1046,28 +1041,24 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
+      <c r="A33" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="B34" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B35" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated naming conventions of database
</commit_message>
<xml_diff>
--- a/assets/design/database.xlsx
+++ b/assets/design/database.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,21 +62,12 @@
     <t>contact_info</t>
   </si>
   <si>
-    <t>crisisID</t>
-  </si>
-  <si>
-    <t>Crisis</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
     <t>Organization</t>
   </si>
   <si>
-    <t>CrisisPerson</t>
-  </si>
-  <si>
     <t>varchar(255) not null foreign key</t>
   </si>
   <si>
@@ -86,18 +77,12 @@
     <t>organizationID</t>
   </si>
   <si>
-    <t>CrisisOrganization</t>
-  </si>
-  <si>
     <t>PersonOrganization</t>
   </si>
   <si>
     <t>Citation</t>
   </si>
   <si>
-    <t>CitationCrisis</t>
-  </si>
-  <si>
     <t>citationID</t>
   </si>
   <si>
@@ -113,9 +98,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>LinkCrisis</t>
-  </si>
-  <si>
     <t>LinkPerson</t>
   </si>
   <si>
@@ -140,9 +122,6 @@
     <t>html</t>
   </si>
   <si>
-    <t>EmbedCrisis</t>
-  </si>
-  <si>
     <t>embedID</t>
   </si>
   <si>
@@ -168,6 +147,27 @@
   </si>
   <si>
     <t>datetime not null</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>EventPerson</t>
+  </si>
+  <si>
+    <t>EventOrganization</t>
+  </si>
+  <si>
+    <t>eventID</t>
+  </si>
+  <si>
+    <t>CitationEvent</t>
+  </si>
+  <si>
+    <t>LinkEvent</t>
+  </si>
+  <si>
+    <t>EmbedEvent</t>
   </si>
 </sst>
 </file>
@@ -574,9 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -590,18 +588,18 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B1" s="2"/>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E1" s="2"/>
       <c r="G1" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -615,10 +613,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2"/>
     </row>
@@ -639,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -652,10 +650,10 @@
       <c r="D4" s="3"/>
       <c r="E4" s="4"/>
       <c r="G4" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -666,11 +664,11 @@
         <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E5" s="4"/>
       <c r="G5" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>7</v>
@@ -678,16 +676,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
@@ -700,13 +698,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H7" s="4"/>
     </row>
@@ -720,10 +718,10 @@
       <c r="D8" s="3"/>
       <c r="E8" s="4"/>
       <c r="G8" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -734,14 +732,14 @@
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4"/>
       <c r="G9" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,10 +750,10 @@
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="4"/>
@@ -764,28 +762,28 @@
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="4"/>
       <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="G12" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -796,14 +794,14 @@
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E13" s="4"/>
       <c r="G13" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -814,10 +812,10 @@
         <v>5</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
@@ -830,13 +828,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H15" s="4"/>
     </row>
@@ -848,35 +846,35 @@
         <v>5</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="D17" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4"/>
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -891,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -926,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="E22" s="4"/>
     </row>
@@ -938,23 +936,23 @@
         <v>5</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D24" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2"/>
       <c r="D25" s="3"/>
@@ -962,43 +960,43 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="D28" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B29" s="4"/>
       <c r="D29" s="3"/>
@@ -1006,60 +1004,60 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E30" s="4"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="4"/>
       <c r="D32" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>